<commit_message>
fix(evaluation): Fix PRD detection and improve student reports
- Fix PRD document detection to handle files starting with PRD_ (e.g., PRD_Route_Enrichment_Tour_Guide_System.md)
- Update EXTRACTION.md to include PRD_*.md pattern
- Fix module import path in run_evaluation.py
- Add generate_student_reports.py script
- Improve student reports to be black box (hide grading methodology):
  * Remove criteria achieved statistics
  * Remove rarity bonus disclosure
  * Remove prevalence percentages
  * Show only final score and actionable feedback
- Regenerate all student reports for WS04, WS05, WS06 with updated format
- Fix grading error for student 87681 and potentially others with non-standard PRD filenames

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/outputs/WorkSubmissions04/grades.xlsx
+++ b/outputs/WorkSubmissions04/grades.xlsx
@@ -484,19 +484,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19.684</v>
+        <v>19.794</v>
       </c>
       <c r="C2" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D2" t="n">
-        <v>95.34973842278629</v>
+        <v>95.37438566059554</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>96.34973842278629</v>
+        <v>96.37438566059554</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -512,19 +512,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>19.684</v>
+        <v>19.794</v>
       </c>
       <c r="C3" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D3" t="n">
-        <v>95.34973842278629</v>
+        <v>95.37438566059554</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>96.34973842278629</v>
+        <v>96.37438566059554</v>
       </c>
       <c r="G3" t="n">
         <v>2</v>
@@ -540,19 +540,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>19.684</v>
+        <v>19.794</v>
       </c>
       <c r="C4" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D4" t="n">
-        <v>95.34973842278629</v>
+        <v>95.37438566059554</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>96.34973842278629</v>
+        <v>96.37438566059554</v>
       </c>
       <c r="G4" t="n">
         <v>3</v>
@@ -568,19 +568,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>18.219</v>
+        <v>18.329</v>
       </c>
       <c r="C5" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D5" t="n">
-        <v>88.2532454950591</v>
+        <v>88.31550544473355</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>89.2532454950591</v>
+        <v>89.31550544473355</v>
       </c>
       <c r="G5" t="n">
         <v>4</v>
@@ -596,19 +596,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>18.219</v>
+        <v>18.329</v>
       </c>
       <c r="C6" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D6" t="n">
-        <v>88.2532454950591</v>
+        <v>88.31550544473355</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>89.2532454950591</v>
+        <v>89.31550544473355</v>
       </c>
       <c r="G6" t="n">
         <v>5</v>
@@ -624,19 +624,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17.959</v>
+        <v>18.069</v>
       </c>
       <c r="C7" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D7" t="n">
-        <v>86.99379965123039</v>
+        <v>87.06273489447817</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>86.99379965123039</v>
+        <v>87.06273489447817</v>
       </c>
       <c r="G7" t="n">
         <v>6</v>
@@ -652,19 +652,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17.959</v>
+        <v>18.069</v>
       </c>
       <c r="C8" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D8" t="n">
-        <v>86.99379965123039</v>
+        <v>87.06273489447817</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>86.99379965123039</v>
+        <v>87.06273489447817</v>
       </c>
       <c r="G8" t="n">
         <v>7</v>
@@ -680,19 +680,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17.029</v>
+        <v>17.139</v>
       </c>
       <c r="C9" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D9" t="n">
-        <v>82.48885874830459</v>
+        <v>82.58167100318011</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>83.48885874830459</v>
+        <v>83.58167100318011</v>
       </c>
       <c r="G9" t="n">
         <v>8</v>
@@ -708,19 +708,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17.029</v>
+        <v>17.139</v>
       </c>
       <c r="C10" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D10" t="n">
-        <v>82.48885874830459</v>
+        <v>82.58167100318011</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>83.48885874830459</v>
+        <v>83.58167100318011</v>
       </c>
       <c r="G10" t="n">
         <v>9</v>
@@ -736,19 +736,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>15.552</v>
+        <v>15.662</v>
       </c>
       <c r="C11" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D11" t="n">
-        <v>75.33423755086224</v>
+        <v>75.46497060807555</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>75.33423755086224</v>
+        <v>75.46497060807555</v>
       </c>
       <c r="G11" t="n">
         <v>10</v>
@@ -764,19 +764,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>15.552</v>
+        <v>15.662</v>
       </c>
       <c r="C12" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D12" t="n">
-        <v>75.33423755086224</v>
+        <v>75.46497060807555</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>75.33423755086224</v>
+        <v>75.46497060807555</v>
       </c>
       <c r="G12" t="n">
         <v>11</v>
@@ -795,16 +795,16 @@
         <v>15.414</v>
       </c>
       <c r="C13" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D13" t="n">
-        <v>74.66576244913777</v>
+        <v>74.27002023706272</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>74.66576244913777</v>
+        <v>74.27002023706272</v>
       </c>
       <c r="G13" t="n">
         <v>12</v>
@@ -820,25 +820,25 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>14.122</v>
+        <v>15.167</v>
       </c>
       <c r="C14" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D14" t="n">
-        <v>68.4072854098043</v>
+        <v>73.07988821432012</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>68.4072854098043</v>
+        <v>73.07988821432012</v>
       </c>
       <c r="G14" t="n">
         <v>13</v>
       </c>
       <c r="H14" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15">
@@ -848,25 +848,25 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>14.122</v>
+        <v>15.167</v>
       </c>
       <c r="C15" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D15" t="n">
-        <v>68.4072854098043</v>
+        <v>73.07988821432012</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>68.4072854098043</v>
+        <v>73.07988821432012</v>
       </c>
       <c r="G15" t="n">
         <v>14</v>
       </c>
       <c r="H15" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16">
@@ -876,19 +876,19 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>13.602</v>
+        <v>13.712</v>
       </c>
       <c r="C16" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D16" t="n">
-        <v>65.88839372214687</v>
+        <v>66.06919148116025</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>65.88839372214687</v>
+        <v>66.06919148116025</v>
       </c>
       <c r="G16" t="n">
         <v>15</v>
@@ -904,19 +904,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>13.602</v>
+        <v>13.712</v>
       </c>
       <c r="C17" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D17" t="n">
-        <v>65.88839372214687</v>
+        <v>66.06919148116025</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>65.88839372214687</v>
+        <v>66.06919148116025</v>
       </c>
       <c r="G17" t="n">
         <v>16</v>
@@ -932,19 +932,19 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>12.609</v>
+        <v>12.719</v>
       </c>
       <c r="C18" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D18" t="n">
-        <v>61.07827940321644</v>
+        <v>61.28457164883877</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>61.07827940321644</v>
+        <v>61.28457164883877</v>
       </c>
       <c r="G18" t="n">
         <v>17</v>
@@ -960,19 +960,19 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>12.072</v>
+        <v>12.182</v>
       </c>
       <c r="C19" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D19" t="n">
-        <v>58.47703933346251</v>
+        <v>58.69711862773441</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>58.47703933346251</v>
+        <v>58.69711862773441</v>
       </c>
       <c r="G19" t="n">
         <v>18</v>
@@ -988,19 +988,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>12.072</v>
+        <v>12.182</v>
       </c>
       <c r="C20" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D20" t="n">
-        <v>58.47703933346251</v>
+        <v>58.69711862773441</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>58.47703933346251</v>
+        <v>58.69711862773441</v>
       </c>
       <c r="G20" t="n">
         <v>19</v>
@@ -1016,19 +1016,19 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>7.025</v>
+        <v>7.135</v>
       </c>
       <c r="C21" t="n">
-        <v>20.644</v>
+        <v>20.754</v>
       </c>
       <c r="D21" t="n">
-        <v>34.02925789575664</v>
+        <v>34.37891490796954</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>34.02925789575664</v>
+        <v>34.37891490796954</v>
       </c>
       <c r="G21" t="n">
         <v>20</v>

</xml_diff>